<commit_message>
Added code till container history tab
</commit_message>
<xml_diff>
--- a/Documentation/Notes.xlsx
+++ b/Documentation/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\PoolCleansingPOC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F652ED8A-674B-4941-9BB1-8005C57CADFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33505AC6-31E3-4183-820B-50C8045C4221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Check for E Records</t>
   </si>
@@ -37,14 +37,79 @@
   </si>
   <si>
     <t>Fetch Details of Earlliest E Record -1</t>
+  </si>
+  <si>
+    <t>Check Container History [R] for Earlliest E Record</t>
+  </si>
+  <si>
+    <t>Check If Trucker Code Changed</t>
+  </si>
+  <si>
+    <t>PIERE</t>
+  </si>
+  <si>
+    <t>GPON</t>
+  </si>
+  <si>
+    <t>LAYTI</t>
+  </si>
+  <si>
+    <t>KRTD</t>
+  </si>
+  <si>
+    <t>BareMove</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>BO- Bare out</t>
+  </si>
+  <si>
+    <t>BI- Bare In</t>
+  </si>
+  <si>
+    <t>Trucker CD</t>
+  </si>
+  <si>
+    <t>Trucker Code Changed</t>
+  </si>
+  <si>
+    <t>10 Mins added to 'E-1' record</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>IG</t>
+  </si>
+  <si>
+    <t>FO - Full out</t>
+  </si>
+  <si>
+    <t>AMPF</t>
+  </si>
+  <si>
+    <t>PMXN</t>
+  </si>
+  <si>
+    <t>Bare Move</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,8 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,40 +422,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.48749999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.6166666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.60972222222222217</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>